<commit_message>
change cell format as text (for numberic id)
</commit_message>
<xml_diff>
--- a/Excelion.xlsx
+++ b/Excelion.xlsx
@@ -178,30 +178,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,17 +493,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="40.625" style="3"/>
-    <col min="3" max="3" width="40.625" style="5"/>
+    <col min="1" max="1" width="33.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="40.625" style="6"/>
+    <col min="3" max="3" width="40.625" style="7"/>
+    <col min="4" max="16384" width="40.625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1"/>

</xml_diff>